<commit_message>
Changes for SOD violation.
</commit_message>
<xml_diff>
--- a/src/data/input/extraction_parameters.xlsx
+++ b/src/data/input/extraction_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moaich\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/monali_aich_capgemini_com/Documents/Desktop/Domains/Workspace/Change_Management/src/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{450E592E-4FB5-4485-ACED-9D51A733744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{450E592E-4FB5-4485-ACED-9D51A733744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E89C657-BB9E-4126-995D-E23F49218AF8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6E39EDFC-DC0D-4EA9-AF92-5E61129AB132}"/>
   </bookViews>
@@ -47,13 +47,13 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>System Type</t>
-  </si>
-  <si>
     <t>Capgemini</t>
   </si>
   <si>
-    <t>ServiceNow</t>
+    <t>Asset Name</t>
+  </si>
+  <si>
+    <t>Warehouse Management System</t>
   </si>
 </sst>
 </file>
@@ -438,15 +438,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" customWidth="1"/>
-    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+    <col min="2" max="2" width="19.90625" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" customWidth="1"/>
+    <col min="4" max="4" width="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -460,18 +460,18 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>45684.397916666669</v>
+        <v>45690.397916666669</v>
       </c>
       <c r="C2" s="2">
-        <v>45687.518055555556</v>
+        <v>45693.791666666664</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -480,4 +480,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{e760c494-6550-44b4-8258-77c175d778b7}" enabled="1" method="Privileged" siteId="{76a2ae5a-9f00-4f6b-95ed-5d33d77c4d61}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
SOD Violation changes  & Unauthorized Approver changes
UI changes for SOD Violation & Not UI change for Unauthorized Approver.
</commit_message>
<xml_diff>
--- a/src/data/input/extraction_parameters.xlsx
+++ b/src/data/input/extraction_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://capgemini-my.sharepoint.com/personal/monali_aich_capgemini_com/Documents/Desktop/Domains/Workspace/Change_Management/src/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{450E592E-4FB5-4485-ACED-9D51A733744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E89C657-BB9E-4126-995D-E23F49218AF8}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{450E592E-4FB5-4485-ACED-9D51A733744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA65A02C-84AF-404C-96BE-048F59AE54EA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6E39EDFC-DC0D-4EA9-AF92-5E61129AB132}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Client Name</t>
   </si>
@@ -47,13 +47,7 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>Capgemini</t>
-  </si>
-  <si>
     <t>Asset Name</t>
-  </si>
-  <si>
-    <t>Warehouse Management System</t>
   </si>
 </sst>
 </file>
@@ -95,12 +89,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4AF5B67-455A-4538-99BA-AA708F98CBD0}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -460,21 +453,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>45690.397916666669</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45693.791666666664</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>